<commit_message>
update Signed-off-by: huuphamlc <huuphamlc@gmail.com>
</commit_message>
<xml_diff>
--- a/WIP/Documents/F_Taxi_UserCaseList_v1.1.xlsx
+++ b/WIP/Documents/F_Taxi_UserCaseList_v1.1.xlsx
@@ -351,10 +351,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -366,8 +369,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +683,7 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
@@ -692,10 +695,10 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -706,8 +709,8 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
@@ -716,8 +719,8 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
@@ -726,8 +729,8 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -738,8 +741,8 @@
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
@@ -748,8 +751,8 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
@@ -758,8 +761,8 @@
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -770,8 +773,8 @@
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
@@ -780,8 +783,8 @@
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="2" t="s">
         <v>52</v>
       </c>
@@ -790,8 +793,8 @@
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="2" t="s">
         <v>76</v>
       </c>
@@ -800,7 +803,7 @@
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>60</v>
@@ -810,7 +813,7 @@
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>61</v>
@@ -820,8 +823,8 @@
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="2" t="s">
         <v>77</v>
       </c>
@@ -830,8 +833,8 @@
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -842,8 +845,8 @@
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
@@ -852,8 +855,8 @@
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="2" t="s">
         <v>55</v>
       </c>
@@ -862,8 +865,8 @@
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="2" t="s">
         <v>62</v>
       </c>
@@ -872,8 +875,8 @@
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="2" t="s">
         <v>63</v>
       </c>
@@ -882,10 +885,10 @@
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -896,8 +899,8 @@
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
@@ -906,8 +909,8 @@
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="2" t="s">
         <v>10</v>
       </c>
@@ -916,8 +919,8 @@
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -928,8 +931,8 @@
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
         <v>14</v>
       </c>
@@ -938,8 +941,8 @@
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="2" t="s">
         <v>12</v>
       </c>
@@ -948,7 +951,7 @@
       <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>17</v>
@@ -958,8 +961,8 @@
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="5"/>
+      <c r="C28" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -970,8 +973,8 @@
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="2" t="s">
         <v>65</v>
       </c>
@@ -980,8 +983,8 @@
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="2" t="s">
         <v>66</v>
       </c>
@@ -990,7 +993,7 @@
       <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
         <v>67</v>
@@ -1000,7 +1003,7 @@
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>68</v>
@@ -1010,8 +1013,8 @@
       <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="3" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1022,8 +1025,8 @@
       <c r="A34" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="2" t="s">
         <v>69</v>
       </c>
@@ -1032,8 +1035,8 @@
       <c r="A35" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="2" t="s">
         <v>30</v>
       </c>
@@ -1042,8 +1045,8 @@
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="2" t="s">
         <v>28</v>
       </c>
@@ -1052,8 +1055,8 @@
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
       <c r="D37" s="2" t="s">
         <v>32</v>
       </c>
@@ -1062,8 +1065,8 @@
       <c r="A38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
       <c r="D38" s="2" t="s">
         <v>62</v>
       </c>

</xml_diff>